<commit_message>
Tables of results almost done
</commit_message>
<xml_diff>
--- a/AllResults_Table -cw1.xlsx
+++ b/AllResults_Table -cw1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Desktop\Università\Year 4\Concurrent of Parrallel Systems\Coursework1\CPS-Coursework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Desktop\Università\Year 4\Concurrent of Parrallel Systems\Coursework2\CPS-Coursework\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1158,24 +1158,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="13" xfId="27" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="16" xfId="27" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="18" xfId="27" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="22" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="23" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="24" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="13" borderId="22" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1206,41 +1188,23 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="22" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="23" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="24" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="13" xfId="27" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="16" xfId="27" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="18" xfId="27" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1264,6 +1228,42 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -18784,7 +18784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G166"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -18799,15 +18799,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="99"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="93"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="17"/>
@@ -18824,8 +18824,8 @@
     <row r="5" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="17"/>
       <c r="B5" s="17"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="100"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
     </row>
     <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
@@ -18851,16 +18851,16 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="88" t="s">
+      <c r="A7" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="91">
+      <c r="B7" s="85">
         <v>9</v>
       </c>
-      <c r="C7" s="94">
+      <c r="C7" s="88">
         <v>400</v>
       </c>
-      <c r="D7" s="85" t="s">
+      <c r="D7" s="98" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="35">
@@ -18874,10 +18874,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="89"/>
-      <c r="B8" s="92"/>
-      <c r="C8" s="95"/>
-      <c r="D8" s="86"/>
+      <c r="A8" s="96"/>
+      <c r="B8" s="86"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="99"/>
       <c r="E8" s="24">
         <v>16</v>
       </c>
@@ -18889,10 +18889,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="89"/>
-      <c r="B9" s="92"/>
-      <c r="C9" s="95"/>
-      <c r="D9" s="86"/>
+      <c r="A9" s="96"/>
+      <c r="B9" s="86"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="99"/>
       <c r="E9" s="24">
         <v>64</v>
       </c>
@@ -18904,10 +18904,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="89"/>
-      <c r="B10" s="92"/>
-      <c r="C10" s="95"/>
-      <c r="D10" s="87"/>
+      <c r="A10" s="96"/>
+      <c r="B10" s="86"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="100"/>
       <c r="E10" s="26">
         <v>256</v>
       </c>
@@ -18919,19 +18919,19 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="89"/>
-      <c r="B11" s="92"/>
-      <c r="C11" s="95"/>
+      <c r="A11" s="96"/>
+      <c r="B11" s="86"/>
+      <c r="C11" s="89"/>
       <c r="D11" s="16"/>
       <c r="E11" s="24"/>
       <c r="F11" s="8"/>
       <c r="G11" s="28"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="89"/>
-      <c r="B12" s="92"/>
-      <c r="C12" s="95"/>
-      <c r="D12" s="85" t="s">
+      <c r="A12" s="96"/>
+      <c r="B12" s="86"/>
+      <c r="C12" s="89"/>
+      <c r="D12" s="98" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="35">
@@ -18945,10 +18945,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="89"/>
-      <c r="B13" s="92"/>
-      <c r="C13" s="95"/>
-      <c r="D13" s="86"/>
+      <c r="A13" s="96"/>
+      <c r="B13" s="86"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="99"/>
       <c r="E13" s="24">
         <v>16</v>
       </c>
@@ -18960,10 +18960,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="89"/>
-      <c r="B14" s="92"/>
-      <c r="C14" s="95"/>
-      <c r="D14" s="86"/>
+      <c r="A14" s="96"/>
+      <c r="B14" s="86"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="99"/>
       <c r="E14" s="24">
         <v>64</v>
       </c>
@@ -18975,10 +18975,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="89"/>
-      <c r="B15" s="92"/>
-      <c r="C15" s="96"/>
-      <c r="D15" s="87"/>
+      <c r="A15" s="96"/>
+      <c r="B15" s="86"/>
+      <c r="C15" s="90"/>
+      <c r="D15" s="100"/>
       <c r="E15" s="26">
         <v>256</v>
       </c>
@@ -18990,8 +18990,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="89"/>
-      <c r="B16" s="92"/>
+      <c r="A16" s="96"/>
+      <c r="B16" s="86"/>
       <c r="C16" s="18"/>
       <c r="D16" s="16"/>
       <c r="E16" s="24"/>
@@ -18999,12 +18999,12 @@
       <c r="G16" s="28"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="89"/>
-      <c r="B17" s="92"/>
-      <c r="C17" s="94">
+      <c r="A17" s="96"/>
+      <c r="B17" s="86"/>
+      <c r="C17" s="88">
         <v>1024</v>
       </c>
-      <c r="D17" s="85" t="s">
+      <c r="D17" s="98" t="s">
         <v>3</v>
       </c>
       <c r="E17" s="35">
@@ -19018,10 +19018,10 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="89"/>
-      <c r="B18" s="92"/>
-      <c r="C18" s="95"/>
-      <c r="D18" s="86"/>
+      <c r="A18" s="96"/>
+      <c r="B18" s="86"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="99"/>
       <c r="E18" s="24">
         <v>16</v>
       </c>
@@ -19033,10 +19033,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="89"/>
-      <c r="B19" s="92"/>
-      <c r="C19" s="95"/>
-      <c r="D19" s="86"/>
+      <c r="A19" s="96"/>
+      <c r="B19" s="86"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="99"/>
       <c r="E19" s="24">
         <v>64</v>
       </c>
@@ -19048,10 +19048,10 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="89"/>
-      <c r="B20" s="92"/>
-      <c r="C20" s="95"/>
-      <c r="D20" s="87"/>
+      <c r="A20" s="96"/>
+      <c r="B20" s="86"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="100"/>
       <c r="E20" s="26">
         <v>256</v>
       </c>
@@ -19063,19 +19063,19 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="89"/>
-      <c r="B21" s="92"/>
-      <c r="C21" s="95"/>
+      <c r="A21" s="96"/>
+      <c r="B21" s="86"/>
+      <c r="C21" s="89"/>
       <c r="D21" s="16"/>
       <c r="E21" s="24"/>
       <c r="F21" s="8"/>
       <c r="G21" s="28"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="89"/>
-      <c r="B22" s="92"/>
-      <c r="C22" s="95"/>
-      <c r="D22" s="85" t="s">
+      <c r="A22" s="96"/>
+      <c r="B22" s="86"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="98" t="s">
         <v>6</v>
       </c>
       <c r="E22" s="35">
@@ -19089,10 +19089,10 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="89"/>
-      <c r="B23" s="92"/>
-      <c r="C23" s="95"/>
-      <c r="D23" s="86"/>
+      <c r="A23" s="96"/>
+      <c r="B23" s="86"/>
+      <c r="C23" s="89"/>
+      <c r="D23" s="99"/>
       <c r="E23" s="24">
         <v>16</v>
       </c>
@@ -19104,10 +19104,10 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="89"/>
-      <c r="B24" s="92"/>
-      <c r="C24" s="95"/>
-      <c r="D24" s="86"/>
+      <c r="A24" s="96"/>
+      <c r="B24" s="86"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="99"/>
       <c r="E24" s="24">
         <v>64</v>
       </c>
@@ -19119,10 +19119,10 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="89"/>
-      <c r="B25" s="93"/>
-      <c r="C25" s="96"/>
-      <c r="D25" s="87"/>
+      <c r="A25" s="96"/>
+      <c r="B25" s="87"/>
+      <c r="C25" s="90"/>
+      <c r="D25" s="100"/>
       <c r="E25" s="26">
         <v>256</v>
       </c>
@@ -19134,7 +19134,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="89"/>
+      <c r="A26" s="96"/>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
       <c r="D26" s="1"/>
@@ -19143,14 +19143,14 @@
       <c r="G26" s="42"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="89"/>
-      <c r="B27" s="91">
+      <c r="A27" s="96"/>
+      <c r="B27" s="85">
         <v>14</v>
       </c>
-      <c r="C27" s="94">
+      <c r="C27" s="88">
         <v>400</v>
       </c>
-      <c r="D27" s="85" t="s">
+      <c r="D27" s="98" t="s">
         <v>3</v>
       </c>
       <c r="E27" s="35">
@@ -19164,10 +19164,10 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="89"/>
-      <c r="B28" s="92"/>
-      <c r="C28" s="95"/>
-      <c r="D28" s="86"/>
+      <c r="A28" s="96"/>
+      <c r="B28" s="86"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="99"/>
       <c r="E28" s="24">
         <v>16</v>
       </c>
@@ -19179,10 +19179,10 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="89"/>
-      <c r="B29" s="92"/>
-      <c r="C29" s="95"/>
-      <c r="D29" s="86"/>
+      <c r="A29" s="96"/>
+      <c r="B29" s="86"/>
+      <c r="C29" s="89"/>
+      <c r="D29" s="99"/>
       <c r="E29" s="24">
         <v>64</v>
       </c>
@@ -19194,10 +19194,10 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="89"/>
-      <c r="B30" s="92"/>
-      <c r="C30" s="95"/>
-      <c r="D30" s="87"/>
+      <c r="A30" s="96"/>
+      <c r="B30" s="86"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="100"/>
       <c r="E30" s="26">
         <v>256</v>
       </c>
@@ -19209,19 +19209,19 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="89"/>
-      <c r="B31" s="92"/>
-      <c r="C31" s="95"/>
+      <c r="A31" s="96"/>
+      <c r="B31" s="86"/>
+      <c r="C31" s="89"/>
       <c r="D31" s="16"/>
       <c r="E31" s="24"/>
       <c r="F31" s="8"/>
       <c r="G31" s="42"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="89"/>
-      <c r="B32" s="92"/>
-      <c r="C32" s="95"/>
-      <c r="D32" s="85" t="s">
+      <c r="A32" s="96"/>
+      <c r="B32" s="86"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="98" t="s">
         <v>6</v>
       </c>
       <c r="E32" s="35">
@@ -19235,10 +19235,10 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="89"/>
-      <c r="B33" s="92"/>
-      <c r="C33" s="95"/>
-      <c r="D33" s="86"/>
+      <c r="A33" s="96"/>
+      <c r="B33" s="86"/>
+      <c r="C33" s="89"/>
+      <c r="D33" s="99"/>
       <c r="E33" s="24">
         <v>16</v>
       </c>
@@ -19250,10 +19250,10 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="89"/>
-      <c r="B34" s="92"/>
-      <c r="C34" s="95"/>
-      <c r="D34" s="86"/>
+      <c r="A34" s="96"/>
+      <c r="B34" s="86"/>
+      <c r="C34" s="89"/>
+      <c r="D34" s="99"/>
       <c r="E34" s="24">
         <v>64</v>
       </c>
@@ -19265,10 +19265,10 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="89"/>
-      <c r="B35" s="93"/>
-      <c r="C35" s="96"/>
-      <c r="D35" s="87"/>
+      <c r="A35" s="96"/>
+      <c r="B35" s="87"/>
+      <c r="C35" s="90"/>
+      <c r="D35" s="100"/>
       <c r="E35" s="26">
         <v>256</v>
       </c>
@@ -19280,7 +19280,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="89"/>
+      <c r="A36" s="96"/>
       <c r="B36" s="19"/>
       <c r="C36" s="19"/>
       <c r="D36" s="16"/>
@@ -19289,14 +19289,14 @@
       <c r="G36" s="42"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="89"/>
-      <c r="B37" s="91">
+      <c r="A37" s="96"/>
+      <c r="B37" s="85">
         <v>20</v>
       </c>
-      <c r="C37" s="94">
+      <c r="C37" s="88">
         <v>400</v>
       </c>
-      <c r="D37" s="85" t="s">
+      <c r="D37" s="98" t="s">
         <v>3</v>
       </c>
       <c r="E37" s="35">
@@ -19310,10 +19310,10 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="89"/>
-      <c r="B38" s="92"/>
-      <c r="C38" s="95"/>
-      <c r="D38" s="86"/>
+      <c r="A38" s="96"/>
+      <c r="B38" s="86"/>
+      <c r="C38" s="89"/>
+      <c r="D38" s="99"/>
       <c r="E38" s="24">
         <v>16</v>
       </c>
@@ -19325,10 +19325,10 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="89"/>
-      <c r="B39" s="92"/>
-      <c r="C39" s="95"/>
-      <c r="D39" s="86"/>
+      <c r="A39" s="96"/>
+      <c r="B39" s="86"/>
+      <c r="C39" s="89"/>
+      <c r="D39" s="99"/>
       <c r="E39" s="24">
         <v>64</v>
       </c>
@@ -19340,10 +19340,10 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="89"/>
-      <c r="B40" s="92"/>
-      <c r="C40" s="95"/>
-      <c r="D40" s="87"/>
+      <c r="A40" s="96"/>
+      <c r="B40" s="86"/>
+      <c r="C40" s="89"/>
+      <c r="D40" s="100"/>
       <c r="E40" s="26">
         <v>256</v>
       </c>
@@ -19355,19 +19355,19 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="89"/>
-      <c r="B41" s="92"/>
-      <c r="C41" s="95"/>
+      <c r="A41" s="96"/>
+      <c r="B41" s="86"/>
+      <c r="C41" s="89"/>
       <c r="D41" s="16"/>
       <c r="E41" s="24"/>
       <c r="F41" s="8"/>
       <c r="G41" s="42"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="89"/>
-      <c r="B42" s="92"/>
-      <c r="C42" s="95"/>
-      <c r="D42" s="85" t="s">
+      <c r="A42" s="96"/>
+      <c r="B42" s="86"/>
+      <c r="C42" s="89"/>
+      <c r="D42" s="98" t="s">
         <v>6</v>
       </c>
       <c r="E42" s="5">
@@ -19381,10 +19381,10 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="89"/>
-      <c r="B43" s="92"/>
-      <c r="C43" s="95"/>
-      <c r="D43" s="86"/>
+      <c r="A43" s="96"/>
+      <c r="B43" s="86"/>
+      <c r="C43" s="89"/>
+      <c r="D43" s="99"/>
       <c r="E43" s="8">
         <v>16</v>
       </c>
@@ -19396,10 +19396,10 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="89"/>
-      <c r="B44" s="92"/>
-      <c r="C44" s="95"/>
-      <c r="D44" s="86"/>
+      <c r="A44" s="96"/>
+      <c r="B44" s="86"/>
+      <c r="C44" s="89"/>
+      <c r="D44" s="99"/>
       <c r="E44" s="8">
         <v>64</v>
       </c>
@@ -19411,10 +19411,10 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="90"/>
-      <c r="B45" s="93"/>
-      <c r="C45" s="96"/>
-      <c r="D45" s="87"/>
+      <c r="A45" s="97"/>
+      <c r="B45" s="87"/>
+      <c r="C45" s="90"/>
+      <c r="D45" s="100"/>
       <c r="E45" s="12">
         <v>256</v>
       </c>
@@ -19434,16 +19434,16 @@
       <c r="G46" s="42"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="88" t="s">
+      <c r="A47" s="95" t="s">
         <v>16</v>
       </c>
-      <c r="B47" s="91">
+      <c r="B47" s="85">
         <v>9</v>
       </c>
-      <c r="C47" s="94">
+      <c r="C47" s="88">
         <v>400</v>
       </c>
-      <c r="D47" s="85" t="s">
+      <c r="D47" s="98" t="s">
         <v>3</v>
       </c>
       <c r="E47" s="35">
@@ -19457,10 +19457,10 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="89"/>
-      <c r="B48" s="92"/>
-      <c r="C48" s="95"/>
-      <c r="D48" s="86"/>
+      <c r="A48" s="96"/>
+      <c r="B48" s="86"/>
+      <c r="C48" s="89"/>
+      <c r="D48" s="99"/>
       <c r="E48" s="24">
         <v>16</v>
       </c>
@@ -19472,10 +19472,10 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="89"/>
-      <c r="B49" s="92"/>
-      <c r="C49" s="95"/>
-      <c r="D49" s="86"/>
+      <c r="A49" s="96"/>
+      <c r="B49" s="86"/>
+      <c r="C49" s="89"/>
+      <c r="D49" s="99"/>
       <c r="E49" s="24">
         <v>64</v>
       </c>
@@ -19487,10 +19487,10 @@
       </c>
     </row>
     <row r="50" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="89"/>
-      <c r="B50" s="92"/>
-      <c r="C50" s="95"/>
-      <c r="D50" s="87"/>
+      <c r="A50" s="96"/>
+      <c r="B50" s="86"/>
+      <c r="C50" s="89"/>
+      <c r="D50" s="100"/>
       <c r="E50" s="26">
         <v>256</v>
       </c>
@@ -19502,19 +19502,19 @@
       </c>
     </row>
     <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="89"/>
-      <c r="B51" s="92"/>
-      <c r="C51" s="95"/>
+      <c r="A51" s="96"/>
+      <c r="B51" s="86"/>
+      <c r="C51" s="89"/>
       <c r="D51" s="16"/>
       <c r="E51" s="24"/>
       <c r="F51" s="8"/>
       <c r="G51" s="42"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="89"/>
-      <c r="B52" s="92"/>
-      <c r="C52" s="95"/>
-      <c r="D52" s="85" t="s">
+      <c r="A52" s="96"/>
+      <c r="B52" s="86"/>
+      <c r="C52" s="89"/>
+      <c r="D52" s="98" t="s">
         <v>6</v>
       </c>
       <c r="E52" s="35">
@@ -19528,10 +19528,10 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="89"/>
-      <c r="B53" s="92"/>
-      <c r="C53" s="95"/>
-      <c r="D53" s="86"/>
+      <c r="A53" s="96"/>
+      <c r="B53" s="86"/>
+      <c r="C53" s="89"/>
+      <c r="D53" s="99"/>
       <c r="E53" s="24">
         <v>16</v>
       </c>
@@ -19543,10 +19543,10 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="89"/>
-      <c r="B54" s="92"/>
-      <c r="C54" s="95"/>
-      <c r="D54" s="86"/>
+      <c r="A54" s="96"/>
+      <c r="B54" s="86"/>
+      <c r="C54" s="89"/>
+      <c r="D54" s="99"/>
       <c r="E54" s="24">
         <v>64</v>
       </c>
@@ -19558,10 +19558,10 @@
       </c>
     </row>
     <row r="55" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="89"/>
-      <c r="B55" s="92"/>
-      <c r="C55" s="96"/>
-      <c r="D55" s="87"/>
+      <c r="A55" s="96"/>
+      <c r="B55" s="86"/>
+      <c r="C55" s="90"/>
+      <c r="D55" s="100"/>
       <c r="E55" s="26">
         <v>256</v>
       </c>
@@ -19573,8 +19573,8 @@
       </c>
     </row>
     <row r="56" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="89"/>
-      <c r="B56" s="92"/>
+      <c r="A56" s="96"/>
+      <c r="B56" s="86"/>
       <c r="C56" s="19"/>
       <c r="D56" s="16"/>
       <c r="E56" s="24"/>
@@ -19582,12 +19582,12 @@
       <c r="G56" s="42"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="89"/>
-      <c r="B57" s="92"/>
-      <c r="C57" s="94">
+      <c r="A57" s="96"/>
+      <c r="B57" s="86"/>
+      <c r="C57" s="88">
         <v>1024</v>
       </c>
-      <c r="D57" s="85" t="s">
+      <c r="D57" s="98" t="s">
         <v>3</v>
       </c>
       <c r="E57" s="35">
@@ -19601,10 +19601,10 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="89"/>
-      <c r="B58" s="92"/>
-      <c r="C58" s="95"/>
-      <c r="D58" s="86"/>
+      <c r="A58" s="96"/>
+      <c r="B58" s="86"/>
+      <c r="C58" s="89"/>
+      <c r="D58" s="99"/>
       <c r="E58" s="24">
         <v>16</v>
       </c>
@@ -19616,10 +19616,10 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="89"/>
-      <c r="B59" s="92"/>
-      <c r="C59" s="95"/>
-      <c r="D59" s="86"/>
+      <c r="A59" s="96"/>
+      <c r="B59" s="86"/>
+      <c r="C59" s="89"/>
+      <c r="D59" s="99"/>
       <c r="E59" s="24">
         <v>64</v>
       </c>
@@ -19631,10 +19631,10 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="89"/>
-      <c r="B60" s="92"/>
-      <c r="C60" s="95"/>
-      <c r="D60" s="87"/>
+      <c r="A60" s="96"/>
+      <c r="B60" s="86"/>
+      <c r="C60" s="89"/>
+      <c r="D60" s="100"/>
       <c r="E60" s="26">
         <v>256</v>
       </c>
@@ -19646,19 +19646,19 @@
       </c>
     </row>
     <row r="61" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="89"/>
-      <c r="B61" s="92"/>
-      <c r="C61" s="95"/>
+      <c r="A61" s="96"/>
+      <c r="B61" s="86"/>
+      <c r="C61" s="89"/>
       <c r="D61" s="16"/>
       <c r="E61" s="24"/>
       <c r="F61" s="8"/>
       <c r="G61" s="42"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="89"/>
-      <c r="B62" s="92"/>
-      <c r="C62" s="95"/>
-      <c r="D62" s="85" t="s">
+      <c r="A62" s="96"/>
+      <c r="B62" s="86"/>
+      <c r="C62" s="89"/>
+      <c r="D62" s="98" t="s">
         <v>6</v>
       </c>
       <c r="E62" s="5">
@@ -19672,10 +19672,10 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="89"/>
-      <c r="B63" s="92"/>
-      <c r="C63" s="95"/>
-      <c r="D63" s="86"/>
+      <c r="A63" s="96"/>
+      <c r="B63" s="86"/>
+      <c r="C63" s="89"/>
+      <c r="D63" s="99"/>
       <c r="E63" s="8">
         <v>16</v>
       </c>
@@ -19687,10 +19687,10 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" s="89"/>
-      <c r="B64" s="92"/>
-      <c r="C64" s="95"/>
-      <c r="D64" s="86"/>
+      <c r="A64" s="96"/>
+      <c r="B64" s="86"/>
+      <c r="C64" s="89"/>
+      <c r="D64" s="99"/>
       <c r="E64" s="8">
         <v>64</v>
       </c>
@@ -19702,10 +19702,10 @@
       </c>
     </row>
     <row r="65" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="89"/>
-      <c r="B65" s="93"/>
-      <c r="C65" s="96"/>
-      <c r="D65" s="87"/>
+      <c r="A65" s="96"/>
+      <c r="B65" s="87"/>
+      <c r="C65" s="90"/>
+      <c r="D65" s="100"/>
       <c r="E65" s="12">
         <v>256</v>
       </c>
@@ -19717,7 +19717,7 @@
       </c>
     </row>
     <row r="66" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="89"/>
+      <c r="A66" s="96"/>
       <c r="B66" s="18"/>
       <c r="C66" s="19"/>
       <c r="D66" s="1"/>
@@ -19726,14 +19726,14 @@
       <c r="G66" s="42"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="89"/>
-      <c r="B67" s="91">
+      <c r="A67" s="96"/>
+      <c r="B67" s="85">
         <v>14</v>
       </c>
-      <c r="C67" s="94">
+      <c r="C67" s="88">
         <v>400</v>
       </c>
-      <c r="D67" s="85" t="s">
+      <c r="D67" s="98" t="s">
         <v>3</v>
       </c>
       <c r="E67" s="35">
@@ -19747,10 +19747,10 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="89"/>
-      <c r="B68" s="92"/>
-      <c r="C68" s="95"/>
-      <c r="D68" s="86"/>
+      <c r="A68" s="96"/>
+      <c r="B68" s="86"/>
+      <c r="C68" s="89"/>
+      <c r="D68" s="99"/>
       <c r="E68" s="24">
         <v>16</v>
       </c>
@@ -19762,10 +19762,10 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="89"/>
-      <c r="B69" s="92"/>
-      <c r="C69" s="95"/>
-      <c r="D69" s="86"/>
+      <c r="A69" s="96"/>
+      <c r="B69" s="86"/>
+      <c r="C69" s="89"/>
+      <c r="D69" s="99"/>
       <c r="E69" s="24">
         <v>64</v>
       </c>
@@ -19777,10 +19777,10 @@
       </c>
     </row>
     <row r="70" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="89"/>
-      <c r="B70" s="92"/>
-      <c r="C70" s="95"/>
-      <c r="D70" s="87"/>
+      <c r="A70" s="96"/>
+      <c r="B70" s="86"/>
+      <c r="C70" s="89"/>
+      <c r="D70" s="100"/>
       <c r="E70" s="26">
         <v>256</v>
       </c>
@@ -19792,19 +19792,19 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="89"/>
-      <c r="B71" s="92"/>
-      <c r="C71" s="95"/>
+      <c r="A71" s="96"/>
+      <c r="B71" s="86"/>
+      <c r="C71" s="89"/>
       <c r="D71" s="16"/>
       <c r="E71" s="24"/>
       <c r="F71" s="8"/>
       <c r="G71" s="42"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" s="89"/>
-      <c r="B72" s="92"/>
-      <c r="C72" s="95"/>
-      <c r="D72" s="85" t="s">
+      <c r="A72" s="96"/>
+      <c r="B72" s="86"/>
+      <c r="C72" s="89"/>
+      <c r="D72" s="98" t="s">
         <v>6</v>
       </c>
       <c r="E72" s="35">
@@ -19818,10 +19818,10 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="89"/>
-      <c r="B73" s="92"/>
-      <c r="C73" s="95"/>
-      <c r="D73" s="86"/>
+      <c r="A73" s="96"/>
+      <c r="B73" s="86"/>
+      <c r="C73" s="89"/>
+      <c r="D73" s="99"/>
       <c r="E73" s="24">
         <v>16</v>
       </c>
@@ -19833,10 +19833,10 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" s="89"/>
-      <c r="B74" s="92"/>
-      <c r="C74" s="95"/>
-      <c r="D74" s="86"/>
+      <c r="A74" s="96"/>
+      <c r="B74" s="86"/>
+      <c r="C74" s="89"/>
+      <c r="D74" s="99"/>
       <c r="E74" s="24">
         <v>64</v>
       </c>
@@ -19848,10 +19848,10 @@
       </c>
     </row>
     <row r="75" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="89"/>
-      <c r="B75" s="93"/>
-      <c r="C75" s="96"/>
-      <c r="D75" s="87"/>
+      <c r="A75" s="96"/>
+      <c r="B75" s="87"/>
+      <c r="C75" s="90"/>
+      <c r="D75" s="100"/>
       <c r="E75" s="26">
         <v>256</v>
       </c>
@@ -19863,7 +19863,7 @@
       </c>
     </row>
     <row r="76" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="89"/>
+      <c r="A76" s="96"/>
       <c r="B76" s="19"/>
       <c r="C76" s="19"/>
       <c r="D76" s="16"/>
@@ -19872,14 +19872,14 @@
       <c r="G76" s="42"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A77" s="89"/>
-      <c r="B77" s="91">
+      <c r="A77" s="96"/>
+      <c r="B77" s="85">
         <v>20</v>
       </c>
-      <c r="C77" s="94">
+      <c r="C77" s="88">
         <v>400</v>
       </c>
-      <c r="D77" s="85" t="s">
+      <c r="D77" s="98" t="s">
         <v>3</v>
       </c>
       <c r="E77" s="35">
@@ -19893,10 +19893,10 @@
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A78" s="89"/>
-      <c r="B78" s="92"/>
-      <c r="C78" s="95"/>
-      <c r="D78" s="86"/>
+      <c r="A78" s="96"/>
+      <c r="B78" s="86"/>
+      <c r="C78" s="89"/>
+      <c r="D78" s="99"/>
       <c r="E78" s="24">
         <v>16</v>
       </c>
@@ -19908,10 +19908,10 @@
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A79" s="89"/>
-      <c r="B79" s="92"/>
-      <c r="C79" s="95"/>
-      <c r="D79" s="86"/>
+      <c r="A79" s="96"/>
+      <c r="B79" s="86"/>
+      <c r="C79" s="89"/>
+      <c r="D79" s="99"/>
       <c r="E79" s="24">
         <v>64</v>
       </c>
@@ -19923,10 +19923,10 @@
       </c>
     </row>
     <row r="80" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="89"/>
-      <c r="B80" s="92"/>
-      <c r="C80" s="95"/>
-      <c r="D80" s="87"/>
+      <c r="A80" s="96"/>
+      <c r="B80" s="86"/>
+      <c r="C80" s="89"/>
+      <c r="D80" s="100"/>
       <c r="E80" s="26">
         <v>256</v>
       </c>
@@ -19938,19 +19938,19 @@
       </c>
     </row>
     <row r="81" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="89"/>
-      <c r="B81" s="92"/>
-      <c r="C81" s="95"/>
+      <c r="A81" s="96"/>
+      <c r="B81" s="86"/>
+      <c r="C81" s="89"/>
       <c r="D81" s="16"/>
       <c r="E81" s="24"/>
       <c r="F81" s="8"/>
       <c r="G81" s="42"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A82" s="89"/>
-      <c r="B82" s="92"/>
-      <c r="C82" s="95"/>
-      <c r="D82" s="85" t="s">
+      <c r="A82" s="96"/>
+      <c r="B82" s="86"/>
+      <c r="C82" s="89"/>
+      <c r="D82" s="98" t="s">
         <v>6</v>
       </c>
       <c r="E82" s="35">
@@ -19964,10 +19964,10 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A83" s="89"/>
-      <c r="B83" s="92"/>
-      <c r="C83" s="95"/>
-      <c r="D83" s="86"/>
+      <c r="A83" s="96"/>
+      <c r="B83" s="86"/>
+      <c r="C83" s="89"/>
+      <c r="D83" s="99"/>
       <c r="E83" s="24">
         <v>16</v>
       </c>
@@ -19979,10 +19979,10 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A84" s="89"/>
-      <c r="B84" s="92"/>
-      <c r="C84" s="95"/>
-      <c r="D84" s="86"/>
+      <c r="A84" s="96"/>
+      <c r="B84" s="86"/>
+      <c r="C84" s="89"/>
+      <c r="D84" s="99"/>
       <c r="E84" s="24">
         <v>64</v>
       </c>
@@ -19994,10 +19994,10 @@
       </c>
     </row>
     <row r="85" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="90"/>
-      <c r="B85" s="93"/>
-      <c r="C85" s="96"/>
-      <c r="D85" s="87"/>
+      <c r="A85" s="97"/>
+      <c r="B85" s="87"/>
+      <c r="C85" s="90"/>
+      <c r="D85" s="100"/>
       <c r="E85" s="26">
         <v>256</v>
       </c>
@@ -20018,16 +20018,16 @@
       <c r="G86" s="42"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A87" s="88" t="s">
+      <c r="A87" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="B87" s="91">
+      <c r="B87" s="85">
         <v>9</v>
       </c>
-      <c r="C87" s="94">
+      <c r="C87" s="88">
         <v>400</v>
       </c>
-      <c r="D87" s="85" t="s">
+      <c r="D87" s="98" t="s">
         <v>3</v>
       </c>
       <c r="E87" s="35">
@@ -20041,10 +20041,10 @@
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A88" s="89"/>
-      <c r="B88" s="92"/>
-      <c r="C88" s="95"/>
-      <c r="D88" s="86"/>
+      <c r="A88" s="96"/>
+      <c r="B88" s="86"/>
+      <c r="C88" s="89"/>
+      <c r="D88" s="99"/>
       <c r="E88" s="24">
         <v>16</v>
       </c>
@@ -20056,10 +20056,10 @@
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A89" s="89"/>
-      <c r="B89" s="92"/>
-      <c r="C89" s="95"/>
-      <c r="D89" s="86"/>
+      <c r="A89" s="96"/>
+      <c r="B89" s="86"/>
+      <c r="C89" s="89"/>
+      <c r="D89" s="99"/>
       <c r="E89" s="24">
         <v>64</v>
       </c>
@@ -20071,10 +20071,10 @@
       </c>
     </row>
     <row r="90" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="89"/>
-      <c r="B90" s="92"/>
-      <c r="C90" s="95"/>
-      <c r="D90" s="87"/>
+      <c r="A90" s="96"/>
+      <c r="B90" s="86"/>
+      <c r="C90" s="89"/>
+      <c r="D90" s="100"/>
       <c r="E90" s="26">
         <v>256</v>
       </c>
@@ -20086,19 +20086,19 @@
       </c>
     </row>
     <row r="91" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="89"/>
-      <c r="B91" s="92"/>
-      <c r="C91" s="95"/>
+      <c r="A91" s="96"/>
+      <c r="B91" s="86"/>
+      <c r="C91" s="89"/>
       <c r="D91" s="16"/>
       <c r="E91" s="24"/>
       <c r="F91" s="8"/>
       <c r="G91" s="42"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A92" s="89"/>
-      <c r="B92" s="92"/>
-      <c r="C92" s="95"/>
-      <c r="D92" s="85" t="s">
+      <c r="A92" s="96"/>
+      <c r="B92" s="86"/>
+      <c r="C92" s="89"/>
+      <c r="D92" s="98" t="s">
         <v>6</v>
       </c>
       <c r="E92" s="35">
@@ -20112,10 +20112,10 @@
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A93" s="89"/>
-      <c r="B93" s="92"/>
-      <c r="C93" s="95"/>
-      <c r="D93" s="86"/>
+      <c r="A93" s="96"/>
+      <c r="B93" s="86"/>
+      <c r="C93" s="89"/>
+      <c r="D93" s="99"/>
       <c r="E93" s="24">
         <v>16</v>
       </c>
@@ -20127,10 +20127,10 @@
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A94" s="89"/>
-      <c r="B94" s="92"/>
-      <c r="C94" s="95"/>
-      <c r="D94" s="86"/>
+      <c r="A94" s="96"/>
+      <c r="B94" s="86"/>
+      <c r="C94" s="89"/>
+      <c r="D94" s="99"/>
       <c r="E94" s="24">
         <v>64</v>
       </c>
@@ -20142,10 +20142,10 @@
       </c>
     </row>
     <row r="95" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="89"/>
-      <c r="B95" s="92"/>
-      <c r="C95" s="96"/>
-      <c r="D95" s="87"/>
+      <c r="A95" s="96"/>
+      <c r="B95" s="86"/>
+      <c r="C95" s="90"/>
+      <c r="D95" s="100"/>
       <c r="E95" s="26">
         <v>256</v>
       </c>
@@ -20157,8 +20157,8 @@
       </c>
     </row>
     <row r="96" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="89"/>
-      <c r="B96" s="92"/>
+      <c r="A96" s="96"/>
+      <c r="B96" s="86"/>
       <c r="C96" s="19"/>
       <c r="D96" s="16"/>
       <c r="E96" s="24"/>
@@ -20166,12 +20166,12 @@
       <c r="G96" s="42"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A97" s="89"/>
-      <c r="B97" s="92"/>
-      <c r="C97" s="94">
+      <c r="A97" s="96"/>
+      <c r="B97" s="86"/>
+      <c r="C97" s="88">
         <v>1024</v>
       </c>
-      <c r="D97" s="85" t="s">
+      <c r="D97" s="98" t="s">
         <v>3</v>
       </c>
       <c r="E97" s="35">
@@ -20185,10 +20185,10 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A98" s="89"/>
-      <c r="B98" s="92"/>
-      <c r="C98" s="95"/>
-      <c r="D98" s="86"/>
+      <c r="A98" s="96"/>
+      <c r="B98" s="86"/>
+      <c r="C98" s="89"/>
+      <c r="D98" s="99"/>
       <c r="E98" s="24">
         <v>16</v>
       </c>
@@ -20200,10 +20200,10 @@
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A99" s="89"/>
-      <c r="B99" s="92"/>
-      <c r="C99" s="95"/>
-      <c r="D99" s="86"/>
+      <c r="A99" s="96"/>
+      <c r="B99" s="86"/>
+      <c r="C99" s="89"/>
+      <c r="D99" s="99"/>
       <c r="E99" s="24">
         <v>64</v>
       </c>
@@ -20215,10 +20215,10 @@
       </c>
     </row>
     <row r="100" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="89"/>
-      <c r="B100" s="92"/>
-      <c r="C100" s="95"/>
-      <c r="D100" s="87"/>
+      <c r="A100" s="96"/>
+      <c r="B100" s="86"/>
+      <c r="C100" s="89"/>
+      <c r="D100" s="100"/>
       <c r="E100" s="26">
         <v>256</v>
       </c>
@@ -20230,19 +20230,19 @@
       </c>
     </row>
     <row r="101" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="89"/>
-      <c r="B101" s="92"/>
-      <c r="C101" s="95"/>
+      <c r="A101" s="96"/>
+      <c r="B101" s="86"/>
+      <c r="C101" s="89"/>
       <c r="D101" s="16"/>
       <c r="E101" s="24"/>
       <c r="F101" s="8"/>
       <c r="G101" s="42"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A102" s="89"/>
-      <c r="B102" s="92"/>
-      <c r="C102" s="95"/>
-      <c r="D102" s="85" t="s">
+      <c r="A102" s="96"/>
+      <c r="B102" s="86"/>
+      <c r="C102" s="89"/>
+      <c r="D102" s="98" t="s">
         <v>6</v>
       </c>
       <c r="E102" s="35">
@@ -20256,10 +20256,10 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A103" s="89"/>
-      <c r="B103" s="92"/>
-      <c r="C103" s="95"/>
-      <c r="D103" s="86"/>
+      <c r="A103" s="96"/>
+      <c r="B103" s="86"/>
+      <c r="C103" s="89"/>
+      <c r="D103" s="99"/>
       <c r="E103" s="24">
         <v>16</v>
       </c>
@@ -20271,10 +20271,10 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A104" s="89"/>
-      <c r="B104" s="92"/>
-      <c r="C104" s="95"/>
-      <c r="D104" s="86"/>
+      <c r="A104" s="96"/>
+      <c r="B104" s="86"/>
+      <c r="C104" s="89"/>
+      <c r="D104" s="99"/>
       <c r="E104" s="24">
         <v>64</v>
       </c>
@@ -20286,10 +20286,10 @@
       </c>
     </row>
     <row r="105" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="89"/>
-      <c r="B105" s="93"/>
-      <c r="C105" s="96"/>
-      <c r="D105" s="87"/>
+      <c r="A105" s="96"/>
+      <c r="B105" s="87"/>
+      <c r="C105" s="90"/>
+      <c r="D105" s="100"/>
       <c r="E105" s="26">
         <v>256</v>
       </c>
@@ -20301,7 +20301,7 @@
       </c>
     </row>
     <row r="106" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="89"/>
+      <c r="A106" s="96"/>
       <c r="B106" s="18"/>
       <c r="C106" s="19"/>
       <c r="D106" s="1"/>
@@ -20310,14 +20310,14 @@
       <c r="G106" s="42"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A107" s="89"/>
-      <c r="B107" s="91">
+      <c r="A107" s="96"/>
+      <c r="B107" s="85">
         <v>14</v>
       </c>
-      <c r="C107" s="94">
+      <c r="C107" s="88">
         <v>400</v>
       </c>
-      <c r="D107" s="85" t="s">
+      <c r="D107" s="98" t="s">
         <v>3</v>
       </c>
       <c r="E107" s="35">
@@ -20331,10 +20331,10 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A108" s="89"/>
-      <c r="B108" s="92"/>
-      <c r="C108" s="95"/>
-      <c r="D108" s="86"/>
+      <c r="A108" s="96"/>
+      <c r="B108" s="86"/>
+      <c r="C108" s="89"/>
+      <c r="D108" s="99"/>
       <c r="E108" s="24">
         <v>16</v>
       </c>
@@ -20346,10 +20346,10 @@
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A109" s="89"/>
-      <c r="B109" s="92"/>
-      <c r="C109" s="95"/>
-      <c r="D109" s="86"/>
+      <c r="A109" s="96"/>
+      <c r="B109" s="86"/>
+      <c r="C109" s="89"/>
+      <c r="D109" s="99"/>
       <c r="E109" s="24">
         <v>64</v>
       </c>
@@ -20361,10 +20361,10 @@
       </c>
     </row>
     <row r="110" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="89"/>
-      <c r="B110" s="92"/>
-      <c r="C110" s="95"/>
-      <c r="D110" s="87"/>
+      <c r="A110" s="96"/>
+      <c r="B110" s="86"/>
+      <c r="C110" s="89"/>
+      <c r="D110" s="100"/>
       <c r="E110" s="26">
         <v>256</v>
       </c>
@@ -20376,19 +20376,19 @@
       </c>
     </row>
     <row r="111" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A111" s="89"/>
-      <c r="B111" s="92"/>
-      <c r="C111" s="95"/>
+      <c r="A111" s="96"/>
+      <c r="B111" s="86"/>
+      <c r="C111" s="89"/>
       <c r="D111" s="16"/>
       <c r="E111" s="24"/>
       <c r="F111" s="8"/>
       <c r="G111" s="42"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A112" s="89"/>
-      <c r="B112" s="92"/>
-      <c r="C112" s="95"/>
-      <c r="D112" s="85" t="s">
+      <c r="A112" s="96"/>
+      <c r="B112" s="86"/>
+      <c r="C112" s="89"/>
+      <c r="D112" s="98" t="s">
         <v>6</v>
       </c>
       <c r="E112" s="35">
@@ -20402,10 +20402,10 @@
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A113" s="89"/>
-      <c r="B113" s="92"/>
-      <c r="C113" s="95"/>
-      <c r="D113" s="86"/>
+      <c r="A113" s="96"/>
+      <c r="B113" s="86"/>
+      <c r="C113" s="89"/>
+      <c r="D113" s="99"/>
       <c r="E113" s="24">
         <v>16</v>
       </c>
@@ -20417,10 +20417,10 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A114" s="89"/>
-      <c r="B114" s="92"/>
-      <c r="C114" s="95"/>
-      <c r="D114" s="86"/>
+      <c r="A114" s="96"/>
+      <c r="B114" s="86"/>
+      <c r="C114" s="89"/>
+      <c r="D114" s="99"/>
       <c r="E114" s="24">
         <v>64</v>
       </c>
@@ -20432,10 +20432,10 @@
       </c>
     </row>
     <row r="115" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="89"/>
-      <c r="B115" s="93"/>
-      <c r="C115" s="96"/>
-      <c r="D115" s="87"/>
+      <c r="A115" s="96"/>
+      <c r="B115" s="87"/>
+      <c r="C115" s="90"/>
+      <c r="D115" s="100"/>
       <c r="E115" s="26">
         <v>256</v>
       </c>
@@ -20447,7 +20447,7 @@
       </c>
     </row>
     <row r="116" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="89"/>
+      <c r="A116" s="96"/>
       <c r="B116" s="19"/>
       <c r="C116" s="19"/>
       <c r="D116" s="16"/>
@@ -20456,14 +20456,14 @@
       <c r="G116" s="42"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A117" s="89"/>
-      <c r="B117" s="91">
+      <c r="A117" s="96"/>
+      <c r="B117" s="85">
         <v>20</v>
       </c>
-      <c r="C117" s="94">
+      <c r="C117" s="88">
         <v>400</v>
       </c>
-      <c r="D117" s="85" t="s">
+      <c r="D117" s="98" t="s">
         <v>3</v>
       </c>
       <c r="E117" s="35">
@@ -20477,10 +20477,10 @@
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A118" s="89"/>
-      <c r="B118" s="92"/>
-      <c r="C118" s="95"/>
-      <c r="D118" s="86"/>
+      <c r="A118" s="96"/>
+      <c r="B118" s="86"/>
+      <c r="C118" s="89"/>
+      <c r="D118" s="99"/>
       <c r="E118" s="24">
         <v>16</v>
       </c>
@@ -20492,10 +20492,10 @@
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A119" s="89"/>
-      <c r="B119" s="92"/>
-      <c r="C119" s="95"/>
-      <c r="D119" s="86"/>
+      <c r="A119" s="96"/>
+      <c r="B119" s="86"/>
+      <c r="C119" s="89"/>
+      <c r="D119" s="99"/>
       <c r="E119" s="24">
         <v>64</v>
       </c>
@@ -20507,10 +20507,10 @@
       </c>
     </row>
     <row r="120" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A120" s="89"/>
-      <c r="B120" s="92"/>
-      <c r="C120" s="95"/>
-      <c r="D120" s="87"/>
+      <c r="A120" s="96"/>
+      <c r="B120" s="86"/>
+      <c r="C120" s="89"/>
+      <c r="D120" s="100"/>
       <c r="E120" s="26">
         <v>256</v>
       </c>
@@ -20522,19 +20522,19 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="89"/>
-      <c r="B121" s="92"/>
-      <c r="C121" s="95"/>
+      <c r="A121" s="96"/>
+      <c r="B121" s="86"/>
+      <c r="C121" s="89"/>
       <c r="D121" s="16"/>
       <c r="E121" s="24"/>
       <c r="F121" s="8"/>
       <c r="G121" s="42"/>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A122" s="89"/>
-      <c r="B122" s="92"/>
-      <c r="C122" s="95"/>
-      <c r="D122" s="85" t="s">
+      <c r="A122" s="96"/>
+      <c r="B122" s="86"/>
+      <c r="C122" s="89"/>
+      <c r="D122" s="98" t="s">
         <v>6</v>
       </c>
       <c r="E122" s="35">
@@ -20548,10 +20548,10 @@
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A123" s="89"/>
-      <c r="B123" s="92"/>
-      <c r="C123" s="95"/>
-      <c r="D123" s="86"/>
+      <c r="A123" s="96"/>
+      <c r="B123" s="86"/>
+      <c r="C123" s="89"/>
+      <c r="D123" s="99"/>
       <c r="E123" s="24">
         <v>16</v>
       </c>
@@ -20563,10 +20563,10 @@
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A124" s="89"/>
-      <c r="B124" s="92"/>
-      <c r="C124" s="95"/>
-      <c r="D124" s="86"/>
+      <c r="A124" s="96"/>
+      <c r="B124" s="86"/>
+      <c r="C124" s="89"/>
+      <c r="D124" s="99"/>
       <c r="E124" s="24">
         <v>64</v>
       </c>
@@ -20578,10 +20578,10 @@
       </c>
     </row>
     <row r="125" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A125" s="90"/>
-      <c r="B125" s="93"/>
-      <c r="C125" s="96"/>
-      <c r="D125" s="87"/>
+      <c r="A125" s="97"/>
+      <c r="B125" s="87"/>
+      <c r="C125" s="90"/>
+      <c r="D125" s="100"/>
       <c r="E125" s="26">
         <v>256</v>
       </c>
@@ -20601,16 +20601,16 @@
       <c r="G126" s="24"/>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A127" s="88" t="s">
+      <c r="A127" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="B127" s="91">
+      <c r="B127" s="85">
         <v>9</v>
       </c>
-      <c r="C127" s="94">
+      <c r="C127" s="88">
         <v>400</v>
       </c>
-      <c r="D127" s="85" t="s">
+      <c r="D127" s="98" t="s">
         <v>3</v>
       </c>
       <c r="E127" s="35">
@@ -20624,10 +20624,10 @@
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A128" s="89"/>
-      <c r="B128" s="92"/>
-      <c r="C128" s="95"/>
-      <c r="D128" s="86"/>
+      <c r="A128" s="96"/>
+      <c r="B128" s="86"/>
+      <c r="C128" s="89"/>
+      <c r="D128" s="99"/>
       <c r="E128" s="24">
         <v>16</v>
       </c>
@@ -20639,10 +20639,10 @@
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A129" s="89"/>
-      <c r="B129" s="92"/>
-      <c r="C129" s="95"/>
-      <c r="D129" s="86"/>
+      <c r="A129" s="96"/>
+      <c r="B129" s="86"/>
+      <c r="C129" s="89"/>
+      <c r="D129" s="99"/>
       <c r="E129" s="24">
         <v>64</v>
       </c>
@@ -20654,10 +20654,10 @@
       </c>
     </row>
     <row r="130" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="89"/>
-      <c r="B130" s="92"/>
-      <c r="C130" s="95"/>
-      <c r="D130" s="87"/>
+      <c r="A130" s="96"/>
+      <c r="B130" s="86"/>
+      <c r="C130" s="89"/>
+      <c r="D130" s="100"/>
       <c r="E130" s="26">
         <v>256</v>
       </c>
@@ -20669,19 +20669,19 @@
       </c>
     </row>
     <row r="131" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="89"/>
-      <c r="B131" s="92"/>
-      <c r="C131" s="95"/>
+      <c r="A131" s="96"/>
+      <c r="B131" s="86"/>
+      <c r="C131" s="89"/>
       <c r="D131" s="16"/>
       <c r="E131" s="24"/>
       <c r="F131" s="8"/>
       <c r="G131" s="42"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A132" s="89"/>
-      <c r="B132" s="92"/>
-      <c r="C132" s="95"/>
-      <c r="D132" s="85" t="s">
+      <c r="A132" s="96"/>
+      <c r="B132" s="86"/>
+      <c r="C132" s="89"/>
+      <c r="D132" s="98" t="s">
         <v>6</v>
       </c>
       <c r="E132" s="35">
@@ -20695,10 +20695,10 @@
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A133" s="89"/>
-      <c r="B133" s="92"/>
-      <c r="C133" s="95"/>
-      <c r="D133" s="86"/>
+      <c r="A133" s="96"/>
+      <c r="B133" s="86"/>
+      <c r="C133" s="89"/>
+      <c r="D133" s="99"/>
       <c r="E133" s="24">
         <v>16</v>
       </c>
@@ -20710,10 +20710,10 @@
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A134" s="89"/>
-      <c r="B134" s="92"/>
-      <c r="C134" s="95"/>
-      <c r="D134" s="86"/>
+      <c r="A134" s="96"/>
+      <c r="B134" s="86"/>
+      <c r="C134" s="89"/>
+      <c r="D134" s="99"/>
       <c r="E134" s="24">
         <v>64</v>
       </c>
@@ -20725,10 +20725,10 @@
       </c>
     </row>
     <row r="135" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A135" s="89"/>
-      <c r="B135" s="92"/>
-      <c r="C135" s="96"/>
-      <c r="D135" s="87"/>
+      <c r="A135" s="96"/>
+      <c r="B135" s="86"/>
+      <c r="C135" s="90"/>
+      <c r="D135" s="100"/>
       <c r="E135" s="26">
         <v>256</v>
       </c>
@@ -20740,8 +20740,8 @@
       </c>
     </row>
     <row r="136" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A136" s="89"/>
-      <c r="B136" s="92"/>
+      <c r="A136" s="96"/>
+      <c r="B136" s="86"/>
       <c r="C136" s="19"/>
       <c r="D136" s="16"/>
       <c r="E136" s="24"/>
@@ -20749,12 +20749,12 @@
       <c r="G136" s="42"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A137" s="89"/>
-      <c r="B137" s="92"/>
-      <c r="C137" s="94">
+      <c r="A137" s="96"/>
+      <c r="B137" s="86"/>
+      <c r="C137" s="88">
         <v>1024</v>
       </c>
-      <c r="D137" s="85" t="s">
+      <c r="D137" s="98" t="s">
         <v>3</v>
       </c>
       <c r="E137" s="35">
@@ -20768,10 +20768,10 @@
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A138" s="89"/>
-      <c r="B138" s="92"/>
-      <c r="C138" s="95"/>
-      <c r="D138" s="86"/>
+      <c r="A138" s="96"/>
+      <c r="B138" s="86"/>
+      <c r="C138" s="89"/>
+      <c r="D138" s="99"/>
       <c r="E138" s="24">
         <v>16</v>
       </c>
@@ -20783,10 +20783,10 @@
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A139" s="89"/>
-      <c r="B139" s="92"/>
-      <c r="C139" s="95"/>
-      <c r="D139" s="86"/>
+      <c r="A139" s="96"/>
+      <c r="B139" s="86"/>
+      <c r="C139" s="89"/>
+      <c r="D139" s="99"/>
       <c r="E139" s="24">
         <v>64</v>
       </c>
@@ -20798,10 +20798,10 @@
       </c>
     </row>
     <row r="140" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A140" s="89"/>
-      <c r="B140" s="92"/>
-      <c r="C140" s="95"/>
-      <c r="D140" s="87"/>
+      <c r="A140" s="96"/>
+      <c r="B140" s="86"/>
+      <c r="C140" s="89"/>
+      <c r="D140" s="100"/>
       <c r="E140" s="26">
         <v>256</v>
       </c>
@@ -20813,19 +20813,19 @@
       </c>
     </row>
     <row r="141" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="89"/>
-      <c r="B141" s="92"/>
-      <c r="C141" s="95"/>
+      <c r="A141" s="96"/>
+      <c r="B141" s="86"/>
+      <c r="C141" s="89"/>
       <c r="D141" s="16"/>
       <c r="E141" s="24"/>
       <c r="F141" s="8"/>
       <c r="G141" s="42"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A142" s="89"/>
-      <c r="B142" s="92"/>
-      <c r="C142" s="95"/>
-      <c r="D142" s="85" t="s">
+      <c r="A142" s="96"/>
+      <c r="B142" s="86"/>
+      <c r="C142" s="89"/>
+      <c r="D142" s="98" t="s">
         <v>6</v>
       </c>
       <c r="E142" s="35">
@@ -20839,10 +20839,10 @@
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A143" s="89"/>
-      <c r="B143" s="92"/>
-      <c r="C143" s="95"/>
-      <c r="D143" s="86"/>
+      <c r="A143" s="96"/>
+      <c r="B143" s="86"/>
+      <c r="C143" s="89"/>
+      <c r="D143" s="99"/>
       <c r="E143" s="24">
         <v>16</v>
       </c>
@@ -20854,10 +20854,10 @@
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A144" s="89"/>
-      <c r="B144" s="92"/>
-      <c r="C144" s="95"/>
-      <c r="D144" s="86"/>
+      <c r="A144" s="96"/>
+      <c r="B144" s="86"/>
+      <c r="C144" s="89"/>
+      <c r="D144" s="99"/>
       <c r="E144" s="24">
         <v>64</v>
       </c>
@@ -20869,10 +20869,10 @@
       </c>
     </row>
     <row r="145" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A145" s="89"/>
-      <c r="B145" s="93"/>
-      <c r="C145" s="96"/>
-      <c r="D145" s="87"/>
+      <c r="A145" s="96"/>
+      <c r="B145" s="87"/>
+      <c r="C145" s="90"/>
+      <c r="D145" s="100"/>
       <c r="E145" s="26">
         <v>256</v>
       </c>
@@ -20884,7 +20884,7 @@
       </c>
     </row>
     <row r="146" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A146" s="89"/>
+      <c r="A146" s="96"/>
       <c r="B146" s="18"/>
       <c r="C146" s="19"/>
       <c r="D146" s="1"/>
@@ -20893,14 +20893,14 @@
       <c r="G146" s="42"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A147" s="89"/>
-      <c r="B147" s="91">
+      <c r="A147" s="96"/>
+      <c r="B147" s="85">
         <v>14</v>
       </c>
-      <c r="C147" s="94">
+      <c r="C147" s="88">
         <v>400</v>
       </c>
-      <c r="D147" s="85" t="s">
+      <c r="D147" s="98" t="s">
         <v>3</v>
       </c>
       <c r="E147" s="35">
@@ -20914,10 +20914,10 @@
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A148" s="89"/>
-      <c r="B148" s="92"/>
-      <c r="C148" s="95"/>
-      <c r="D148" s="86"/>
+      <c r="A148" s="96"/>
+      <c r="B148" s="86"/>
+      <c r="C148" s="89"/>
+      <c r="D148" s="99"/>
       <c r="E148" s="24">
         <v>16</v>
       </c>
@@ -20929,10 +20929,10 @@
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A149" s="89"/>
-      <c r="B149" s="92"/>
-      <c r="C149" s="95"/>
-      <c r="D149" s="86"/>
+      <c r="A149" s="96"/>
+      <c r="B149" s="86"/>
+      <c r="C149" s="89"/>
+      <c r="D149" s="99"/>
       <c r="E149" s="24">
         <v>64</v>
       </c>
@@ -20944,10 +20944,10 @@
       </c>
     </row>
     <row r="150" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A150" s="89"/>
-      <c r="B150" s="92"/>
-      <c r="C150" s="95"/>
-      <c r="D150" s="87"/>
+      <c r="A150" s="96"/>
+      <c r="B150" s="86"/>
+      <c r="C150" s="89"/>
+      <c r="D150" s="100"/>
       <c r="E150" s="26">
         <v>256</v>
       </c>
@@ -20959,19 +20959,19 @@
       </c>
     </row>
     <row r="151" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A151" s="89"/>
-      <c r="B151" s="92"/>
-      <c r="C151" s="95"/>
+      <c r="A151" s="96"/>
+      <c r="B151" s="86"/>
+      <c r="C151" s="89"/>
       <c r="D151" s="16"/>
       <c r="E151" s="24"/>
       <c r="F151" s="8"/>
       <c r="G151" s="42"/>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A152" s="89"/>
-      <c r="B152" s="92"/>
-      <c r="C152" s="95"/>
-      <c r="D152" s="85" t="s">
+      <c r="A152" s="96"/>
+      <c r="B152" s="86"/>
+      <c r="C152" s="89"/>
+      <c r="D152" s="98" t="s">
         <v>6</v>
       </c>
       <c r="E152" s="35">
@@ -20985,10 +20985,10 @@
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A153" s="89"/>
-      <c r="B153" s="92"/>
-      <c r="C153" s="95"/>
-      <c r="D153" s="86"/>
+      <c r="A153" s="96"/>
+      <c r="B153" s="86"/>
+      <c r="C153" s="89"/>
+      <c r="D153" s="99"/>
       <c r="E153" s="24">
         <v>16</v>
       </c>
@@ -21000,10 +21000,10 @@
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A154" s="89"/>
-      <c r="B154" s="92"/>
-      <c r="C154" s="95"/>
-      <c r="D154" s="86"/>
+      <c r="A154" s="96"/>
+      <c r="B154" s="86"/>
+      <c r="C154" s="89"/>
+      <c r="D154" s="99"/>
       <c r="E154" s="24">
         <v>64</v>
       </c>
@@ -21015,10 +21015,10 @@
       </c>
     </row>
     <row r="155" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A155" s="89"/>
-      <c r="B155" s="93"/>
-      <c r="C155" s="96"/>
-      <c r="D155" s="87"/>
+      <c r="A155" s="96"/>
+      <c r="B155" s="87"/>
+      <c r="C155" s="90"/>
+      <c r="D155" s="100"/>
       <c r="E155" s="26">
         <v>256</v>
       </c>
@@ -21030,7 +21030,7 @@
       </c>
     </row>
     <row r="156" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A156" s="89"/>
+      <c r="A156" s="96"/>
       <c r="B156" s="19"/>
       <c r="C156" s="19"/>
       <c r="D156" s="16"/>
@@ -21039,14 +21039,14 @@
       <c r="G156" s="42"/>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A157" s="89"/>
-      <c r="B157" s="91">
+      <c r="A157" s="96"/>
+      <c r="B157" s="85">
         <v>20</v>
       </c>
-      <c r="C157" s="94">
+      <c r="C157" s="88">
         <v>400</v>
       </c>
-      <c r="D157" s="85" t="s">
+      <c r="D157" s="98" t="s">
         <v>3</v>
       </c>
       <c r="E157" s="35">
@@ -21060,10 +21060,10 @@
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A158" s="89"/>
-      <c r="B158" s="92"/>
-      <c r="C158" s="95"/>
-      <c r="D158" s="86"/>
+      <c r="A158" s="96"/>
+      <c r="B158" s="86"/>
+      <c r="C158" s="89"/>
+      <c r="D158" s="99"/>
       <c r="E158" s="24">
         <v>16</v>
       </c>
@@ -21075,10 +21075,10 @@
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A159" s="89"/>
-      <c r="B159" s="92"/>
-      <c r="C159" s="95"/>
-      <c r="D159" s="86"/>
+      <c r="A159" s="96"/>
+      <c r="B159" s="86"/>
+      <c r="C159" s="89"/>
+      <c r="D159" s="99"/>
       <c r="E159" s="24">
         <v>64</v>
       </c>
@@ -21090,10 +21090,10 @@
       </c>
     </row>
     <row r="160" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A160" s="89"/>
-      <c r="B160" s="92"/>
-      <c r="C160" s="95"/>
-      <c r="D160" s="87"/>
+      <c r="A160" s="96"/>
+      <c r="B160" s="86"/>
+      <c r="C160" s="89"/>
+      <c r="D160" s="100"/>
       <c r="E160" s="26">
         <v>256</v>
       </c>
@@ -21105,19 +21105,19 @@
       </c>
     </row>
     <row r="161" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A161" s="89"/>
-      <c r="B161" s="92"/>
-      <c r="C161" s="95"/>
+      <c r="A161" s="96"/>
+      <c r="B161" s="86"/>
+      <c r="C161" s="89"/>
       <c r="D161" s="16"/>
       <c r="E161" s="24"/>
       <c r="F161" s="8"/>
       <c r="G161" s="42"/>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A162" s="89"/>
-      <c r="B162" s="92"/>
-      <c r="C162" s="95"/>
-      <c r="D162" s="85" t="s">
+      <c r="A162" s="96"/>
+      <c r="B162" s="86"/>
+      <c r="C162" s="89"/>
+      <c r="D162" s="98" t="s">
         <v>6</v>
       </c>
       <c r="E162" s="35">
@@ -21131,10 +21131,10 @@
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A163" s="89"/>
-      <c r="B163" s="92"/>
-      <c r="C163" s="95"/>
-      <c r="D163" s="86"/>
+      <c r="A163" s="96"/>
+      <c r="B163" s="86"/>
+      <c r="C163" s="89"/>
+      <c r="D163" s="99"/>
       <c r="E163" s="24">
         <v>16</v>
       </c>
@@ -21146,10 +21146,10 @@
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A164" s="89"/>
-      <c r="B164" s="92"/>
-      <c r="C164" s="95"/>
-      <c r="D164" s="86"/>
+      <c r="A164" s="96"/>
+      <c r="B164" s="86"/>
+      <c r="C164" s="89"/>
+      <c r="D164" s="99"/>
       <c r="E164" s="24">
         <v>64</v>
       </c>
@@ -21161,10 +21161,10 @@
       </c>
     </row>
     <row r="165" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A165" s="90"/>
-      <c r="B165" s="93"/>
-      <c r="C165" s="96"/>
-      <c r="D165" s="87"/>
+      <c r="A165" s="97"/>
+      <c r="B165" s="87"/>
+      <c r="C165" s="90"/>
+      <c r="D165" s="100"/>
       <c r="E165" s="26">
         <v>256</v>
       </c>
@@ -21181,6 +21181,56 @@
     </row>
   </sheetData>
   <mergeCells count="66">
+    <mergeCell ref="D157:D160"/>
+    <mergeCell ref="D162:D165"/>
+    <mergeCell ref="D117:D120"/>
+    <mergeCell ref="D122:D125"/>
+    <mergeCell ref="A127:A165"/>
+    <mergeCell ref="B127:B145"/>
+    <mergeCell ref="C127:C135"/>
+    <mergeCell ref="D127:D130"/>
+    <mergeCell ref="D132:D135"/>
+    <mergeCell ref="C137:C145"/>
+    <mergeCell ref="D137:D140"/>
+    <mergeCell ref="D142:D145"/>
+    <mergeCell ref="B147:B155"/>
+    <mergeCell ref="C147:C155"/>
+    <mergeCell ref="D147:D150"/>
+    <mergeCell ref="D152:D155"/>
+    <mergeCell ref="B157:B165"/>
+    <mergeCell ref="C157:C165"/>
+    <mergeCell ref="D77:D80"/>
+    <mergeCell ref="D82:D85"/>
+    <mergeCell ref="A87:A125"/>
+    <mergeCell ref="B87:B105"/>
+    <mergeCell ref="C87:C95"/>
+    <mergeCell ref="D87:D90"/>
+    <mergeCell ref="D92:D95"/>
+    <mergeCell ref="C97:C105"/>
+    <mergeCell ref="D97:D100"/>
+    <mergeCell ref="D102:D105"/>
+    <mergeCell ref="B107:B115"/>
+    <mergeCell ref="C107:C115"/>
+    <mergeCell ref="D107:D110"/>
+    <mergeCell ref="D112:D115"/>
+    <mergeCell ref="A47:A85"/>
+    <mergeCell ref="B47:B65"/>
+    <mergeCell ref="C47:C55"/>
+    <mergeCell ref="D47:D50"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="C57:C65"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="D62:D65"/>
+    <mergeCell ref="B67:B75"/>
+    <mergeCell ref="C67:C75"/>
+    <mergeCell ref="D67:D70"/>
+    <mergeCell ref="D72:D75"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="B117:B125"/>
+    <mergeCell ref="C117:C125"/>
+    <mergeCell ref="D37:D40"/>
+    <mergeCell ref="D42:D45"/>
     <mergeCell ref="B37:B45"/>
     <mergeCell ref="C37:C45"/>
     <mergeCell ref="B77:B85"/>
@@ -21197,56 +21247,6 @@
     <mergeCell ref="D22:D25"/>
     <mergeCell ref="B27:B35"/>
     <mergeCell ref="C27:C35"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="B117:B125"/>
-    <mergeCell ref="C117:C125"/>
-    <mergeCell ref="D37:D40"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="A47:A85"/>
-    <mergeCell ref="B47:B65"/>
-    <mergeCell ref="C47:C55"/>
-    <mergeCell ref="D47:D50"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="C57:C65"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="D62:D65"/>
-    <mergeCell ref="B67:B75"/>
-    <mergeCell ref="C67:C75"/>
-    <mergeCell ref="D67:D70"/>
-    <mergeCell ref="D72:D75"/>
-    <mergeCell ref="B157:B165"/>
-    <mergeCell ref="C157:C165"/>
-    <mergeCell ref="D77:D80"/>
-    <mergeCell ref="D82:D85"/>
-    <mergeCell ref="A87:A125"/>
-    <mergeCell ref="B87:B105"/>
-    <mergeCell ref="C87:C95"/>
-    <mergeCell ref="D87:D90"/>
-    <mergeCell ref="D92:D95"/>
-    <mergeCell ref="C97:C105"/>
-    <mergeCell ref="D97:D100"/>
-    <mergeCell ref="D102:D105"/>
-    <mergeCell ref="B107:B115"/>
-    <mergeCell ref="C107:C115"/>
-    <mergeCell ref="D107:D110"/>
-    <mergeCell ref="D112:D115"/>
-    <mergeCell ref="D157:D160"/>
-    <mergeCell ref="D162:D165"/>
-    <mergeCell ref="D117:D120"/>
-    <mergeCell ref="D122:D125"/>
-    <mergeCell ref="A127:A165"/>
-    <mergeCell ref="B127:B145"/>
-    <mergeCell ref="C127:C135"/>
-    <mergeCell ref="D127:D130"/>
-    <mergeCell ref="D132:D135"/>
-    <mergeCell ref="C137:C145"/>
-    <mergeCell ref="D137:D140"/>
-    <mergeCell ref="D142:D145"/>
-    <mergeCell ref="B147:B155"/>
-    <mergeCell ref="C147:C155"/>
-    <mergeCell ref="D147:D150"/>
-    <mergeCell ref="D152:D155"/>
   </mergeCells>
   <conditionalFormatting sqref="F6">
     <cfRule type="duplicateValues" dxfId="2" priority="4"/>
@@ -21259,8 +21259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A236" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P277" sqref="P277"/>
+    <sheetView tabSelected="1" topLeftCell="A241" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S116" sqref="S116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21322,52 +21322,52 @@
       <c r="U2" s="68"/>
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="101" t="s">
+      <c r="A3" s="115" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="102"/>
-      <c r="K3" s="102"/>
-      <c r="L3" s="102"/>
-      <c r="M3" s="102"/>
-      <c r="N3" s="102"/>
-      <c r="O3" s="102"/>
-      <c r="P3" s="102"/>
-      <c r="Q3" s="102"/>
-      <c r="R3" s="102"/>
-      <c r="S3" s="102"/>
-      <c r="T3" s="102"/>
-      <c r="U3" s="103"/>
+      <c r="B3" s="116"/>
+      <c r="C3" s="116"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="116"/>
+      <c r="F3" s="116"/>
+      <c r="G3" s="116"/>
+      <c r="H3" s="116"/>
+      <c r="I3" s="116"/>
+      <c r="J3" s="116"/>
+      <c r="K3" s="116"/>
+      <c r="L3" s="116"/>
+      <c r="M3" s="116"/>
+      <c r="N3" s="116"/>
+      <c r="O3" s="116"/>
+      <c r="P3" s="116"/>
+      <c r="Q3" s="116"/>
+      <c r="R3" s="116"/>
+      <c r="S3" s="116"/>
+      <c r="T3" s="116"/>
+      <c r="U3" s="117"/>
     </row>
     <row r="4" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="104"/>
-      <c r="B4" s="105"/>
-      <c r="C4" s="105"/>
-      <c r="D4" s="105"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="105"/>
-      <c r="M4" s="105"/>
-      <c r="N4" s="105"/>
-      <c r="O4" s="105"/>
-      <c r="P4" s="105"/>
-      <c r="Q4" s="105"/>
-      <c r="R4" s="105"/>
-      <c r="S4" s="105"/>
-      <c r="T4" s="105"/>
-      <c r="U4" s="106"/>
+      <c r="A4" s="118"/>
+      <c r="B4" s="119"/>
+      <c r="C4" s="119"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
+      <c r="G4" s="119"/>
+      <c r="H4" s="119"/>
+      <c r="I4" s="119"/>
+      <c r="J4" s="119"/>
+      <c r="K4" s="119"/>
+      <c r="L4" s="119"/>
+      <c r="M4" s="119"/>
+      <c r="N4" s="119"/>
+      <c r="O4" s="119"/>
+      <c r="P4" s="119"/>
+      <c r="Q4" s="119"/>
+      <c r="R4" s="119"/>
+      <c r="S4" s="119"/>
+      <c r="T4" s="119"/>
+      <c r="U4" s="120"/>
     </row>
     <row r="29" spans="15:24" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="15:24" x14ac:dyDescent="0.3">
@@ -21592,16 +21592,16 @@
         <v>14</v>
       </c>
       <c r="Q48" s="9"/>
-      <c r="R48" s="116" t="s">
+      <c r="R48" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="S48" s="116"/>
+      <c r="S48" s="104"/>
       <c r="T48" s="9"/>
-      <c r="U48" s="116" t="s">
+      <c r="U48" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="V48" s="116"/>
-      <c r="W48" s="116"/>
+      <c r="V48" s="104"/>
+      <c r="W48" s="104"/>
       <c r="X48" s="10"/>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.3">
@@ -21615,12 +21615,12 @@
       </c>
       <c r="S49" s="9"/>
       <c r="T49" s="9"/>
-      <c r="U49" s="117">
+      <c r="U49" s="105">
         <f>CORREL(P49:P53,R49:R53)</f>
         <v>0.99167354664641849</v>
       </c>
-      <c r="V49" s="117"/>
-      <c r="W49" s="117"/>
+      <c r="V49" s="105"/>
+      <c r="W49" s="105"/>
       <c r="X49" s="10"/>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.3">
@@ -21634,9 +21634,9 @@
       </c>
       <c r="S50" s="9"/>
       <c r="T50" s="9"/>
-      <c r="U50" s="117"/>
-      <c r="V50" s="117"/>
-      <c r="W50" s="117"/>
+      <c r="U50" s="105"/>
+      <c r="V50" s="105"/>
+      <c r="W50" s="105"/>
       <c r="X50" s="10"/>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.3">
@@ -22075,11 +22075,11 @@
       </c>
       <c r="E73" s="9"/>
       <c r="F73" s="9"/>
-      <c r="G73" s="116" t="s">
+      <c r="G73" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="H73" s="116"/>
-      <c r="I73" s="116"/>
+      <c r="H73" s="104"/>
+      <c r="I73" s="104"/>
       <c r="J73" s="10"/>
       <c r="O73" s="8"/>
       <c r="P73" s="15">
@@ -22107,12 +22107,12 @@
       </c>
       <c r="E74" s="9"/>
       <c r="F74" s="9"/>
-      <c r="G74" s="117">
+      <c r="G74" s="105">
         <f>CORREL(B74:B77,D74:D77)</f>
         <v>0.99999886379625136</v>
       </c>
-      <c r="H74" s="117"/>
-      <c r="I74" s="117"/>
+      <c r="H74" s="105"/>
+      <c r="I74" s="105"/>
       <c r="J74" s="10"/>
       <c r="O74" s="8"/>
       <c r="P74" s="15">
@@ -22138,9 +22138,9 @@
       </c>
       <c r="E75" s="9"/>
       <c r="F75" s="9"/>
-      <c r="G75" s="117"/>
-      <c r="H75" s="117"/>
-      <c r="I75" s="117"/>
+      <c r="G75" s="105"/>
+      <c r="H75" s="105"/>
+      <c r="I75" s="105"/>
       <c r="J75" s="10"/>
       <c r="O75" s="8"/>
       <c r="P75" s="9">
@@ -22542,9 +22542,9 @@
       <c r="D100" s="9"/>
       <c r="E100" s="9"/>
       <c r="F100" s="9"/>
-      <c r="G100" s="116"/>
-      <c r="H100" s="116"/>
-      <c r="I100" s="116"/>
+      <c r="G100" s="104"/>
+      <c r="H100" s="104"/>
+      <c r="I100" s="104"/>
       <c r="J100" s="9"/>
       <c r="K100" s="9"/>
       <c r="L100" s="9"/>
@@ -22557,9 +22557,9 @@
       <c r="D101" s="11"/>
       <c r="E101" s="9"/>
       <c r="F101" s="9"/>
-      <c r="G101" s="117"/>
-      <c r="H101" s="117"/>
-      <c r="I101" s="117"/>
+      <c r="G101" s="105"/>
+      <c r="H101" s="105"/>
+      <c r="I101" s="105"/>
       <c r="J101" s="9"/>
       <c r="K101" s="9"/>
       <c r="L101" s="9"/>
@@ -22572,9 +22572,9 @@
       <c r="D102" s="11"/>
       <c r="E102" s="9"/>
       <c r="F102" s="9"/>
-      <c r="G102" s="117"/>
-      <c r="H102" s="117"/>
-      <c r="I102" s="117"/>
+      <c r="G102" s="105"/>
+      <c r="H102" s="105"/>
+      <c r="I102" s="105"/>
       <c r="J102" s="9"/>
       <c r="K102" s="9"/>
       <c r="L102" s="9"/>
@@ -22627,52 +22627,52 @@
     </row>
     <row r="108" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="109" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A109" s="101" t="s">
+      <c r="A109" s="115" t="s">
         <v>22</v>
       </c>
-      <c r="B109" s="102"/>
-      <c r="C109" s="102"/>
-      <c r="D109" s="102"/>
-      <c r="E109" s="102"/>
-      <c r="F109" s="102"/>
-      <c r="G109" s="102"/>
-      <c r="H109" s="102"/>
-      <c r="I109" s="102"/>
-      <c r="J109" s="102"/>
-      <c r="K109" s="102"/>
-      <c r="L109" s="102"/>
-      <c r="M109" s="102"/>
-      <c r="N109" s="102"/>
-      <c r="O109" s="102"/>
-      <c r="P109" s="102"/>
-      <c r="Q109" s="102"/>
-      <c r="R109" s="102"/>
-      <c r="S109" s="102"/>
-      <c r="T109" s="102"/>
-      <c r="U109" s="103"/>
+      <c r="B109" s="116"/>
+      <c r="C109" s="116"/>
+      <c r="D109" s="116"/>
+      <c r="E109" s="116"/>
+      <c r="F109" s="116"/>
+      <c r="G109" s="116"/>
+      <c r="H109" s="116"/>
+      <c r="I109" s="116"/>
+      <c r="J109" s="116"/>
+      <c r="K109" s="116"/>
+      <c r="L109" s="116"/>
+      <c r="M109" s="116"/>
+      <c r="N109" s="116"/>
+      <c r="O109" s="116"/>
+      <c r="P109" s="116"/>
+      <c r="Q109" s="116"/>
+      <c r="R109" s="116"/>
+      <c r="S109" s="116"/>
+      <c r="T109" s="116"/>
+      <c r="U109" s="117"/>
     </row>
     <row r="110" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="104"/>
-      <c r="B110" s="105"/>
-      <c r="C110" s="105"/>
-      <c r="D110" s="105"/>
-      <c r="E110" s="105"/>
-      <c r="F110" s="105"/>
-      <c r="G110" s="105"/>
-      <c r="H110" s="105"/>
-      <c r="I110" s="105"/>
-      <c r="J110" s="105"/>
-      <c r="K110" s="105"/>
-      <c r="L110" s="105"/>
-      <c r="M110" s="105"/>
-      <c r="N110" s="105"/>
-      <c r="O110" s="105"/>
-      <c r="P110" s="105"/>
-      <c r="Q110" s="105"/>
-      <c r="R110" s="105"/>
-      <c r="S110" s="105"/>
-      <c r="T110" s="105"/>
-      <c r="U110" s="106"/>
+      <c r="A110" s="118"/>
+      <c r="B110" s="119"/>
+      <c r="C110" s="119"/>
+      <c r="D110" s="119"/>
+      <c r="E110" s="119"/>
+      <c r="F110" s="119"/>
+      <c r="G110" s="119"/>
+      <c r="H110" s="119"/>
+      <c r="I110" s="119"/>
+      <c r="J110" s="119"/>
+      <c r="K110" s="119"/>
+      <c r="L110" s="119"/>
+      <c r="M110" s="119"/>
+      <c r="N110" s="119"/>
+      <c r="O110" s="119"/>
+      <c r="P110" s="119"/>
+      <c r="Q110" s="119"/>
+      <c r="R110" s="119"/>
+      <c r="S110" s="119"/>
+      <c r="T110" s="119"/>
+      <c r="U110" s="120"/>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A111" s="5"/>
@@ -22737,13 +22737,13 @@
       <c r="N113" s="9"/>
       <c r="O113" s="9"/>
       <c r="P113" s="9"/>
-      <c r="Q113" s="107" t="s">
+      <c r="Q113" s="109" t="s">
         <v>24</v>
       </c>
-      <c r="R113" s="108"/>
-      <c r="S113" s="108"/>
-      <c r="T113" s="108"/>
-      <c r="U113" s="109"/>
+      <c r="R113" s="110"/>
+      <c r="S113" s="110"/>
+      <c r="T113" s="110"/>
+      <c r="U113" s="111"/>
     </row>
     <row r="114" spans="1:21" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A114" s="8"/>
@@ -22763,12 +22763,12 @@
       <c r="O114" s="9"/>
       <c r="P114" s="54"/>
       <c r="Q114" s="58"/>
-      <c r="R114" s="110" t="s">
+      <c r="R114" s="112" t="s">
         <v>25</v>
       </c>
-      <c r="S114" s="111"/>
-      <c r="T114" s="111"/>
-      <c r="U114" s="112"/>
+      <c r="S114" s="113"/>
+      <c r="T114" s="113"/>
+      <c r="U114" s="114"/>
     </row>
     <row r="115" spans="1:21" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A115" s="8"/>
@@ -22787,7 +22787,7 @@
       <c r="N115" s="9"/>
       <c r="O115" s="9"/>
       <c r="P115" s="9"/>
-      <c r="Q115" s="113" t="s">
+      <c r="Q115" s="101" t="s">
         <v>26</v>
       </c>
       <c r="R115" s="65"/>
@@ -22818,7 +22818,7 @@
       <c r="N116" s="9"/>
       <c r="O116" s="9"/>
       <c r="P116" s="9"/>
-      <c r="Q116" s="114"/>
+      <c r="Q116" s="102"/>
       <c r="R116" s="64" t="s">
         <v>27</v>
       </c>
@@ -22852,7 +22852,7 @@
       <c r="N117" s="9"/>
       <c r="O117" s="9"/>
       <c r="P117" s="9"/>
-      <c r="Q117" s="114"/>
+      <c r="Q117" s="102"/>
       <c r="R117" s="59" t="s">
         <v>28</v>
       </c>
@@ -22886,7 +22886,7 @@
       <c r="N118" s="9"/>
       <c r="O118" s="9"/>
       <c r="P118" s="9"/>
-      <c r="Q118" s="115"/>
+      <c r="Q118" s="103"/>
       <c r="R118" s="60" t="s">
         <v>29</v>
       </c>
@@ -22989,13 +22989,13 @@
       <c r="N122" s="9"/>
       <c r="O122" s="9"/>
       <c r="P122" s="9"/>
-      <c r="Q122" s="107" t="s">
+      <c r="Q122" s="109" t="s">
         <v>30</v>
       </c>
-      <c r="R122" s="108"/>
-      <c r="S122" s="108"/>
-      <c r="T122" s="108"/>
-      <c r="U122" s="109"/>
+      <c r="R122" s="110"/>
+      <c r="S122" s="110"/>
+      <c r="T122" s="110"/>
+      <c r="U122" s="111"/>
     </row>
     <row r="123" spans="1:21" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A123" s="8"/>
@@ -23015,12 +23015,12 @@
       <c r="O123" s="9"/>
       <c r="P123" s="9"/>
       <c r="Q123" s="58"/>
-      <c r="R123" s="110" t="s">
+      <c r="R123" s="112" t="s">
         <v>25</v>
       </c>
-      <c r="S123" s="111"/>
-      <c r="T123" s="111"/>
-      <c r="U123" s="112"/>
+      <c r="S123" s="113"/>
+      <c r="T123" s="113"/>
+      <c r="U123" s="114"/>
     </row>
     <row r="124" spans="1:21" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A124" s="8"/>
@@ -23039,7 +23039,7 @@
       <c r="N124" s="9"/>
       <c r="O124" s="9"/>
       <c r="P124" s="9"/>
-      <c r="Q124" s="113" t="s">
+      <c r="Q124" s="101" t="s">
         <v>26</v>
       </c>
       <c r="R124" s="65"/>
@@ -23070,7 +23070,7 @@
       <c r="N125" s="9"/>
       <c r="O125" s="9"/>
       <c r="P125" s="9"/>
-      <c r="Q125" s="114"/>
+      <c r="Q125" s="102"/>
       <c r="R125" s="64" t="s">
         <v>27</v>
       </c>
@@ -23104,7 +23104,7 @@
       <c r="N126" s="9"/>
       <c r="O126" s="9"/>
       <c r="P126" s="9"/>
-      <c r="Q126" s="114"/>
+      <c r="Q126" s="102"/>
       <c r="R126" s="59" t="s">
         <v>28</v>
       </c>
@@ -23138,7 +23138,7 @@
       <c r="N127" s="9"/>
       <c r="O127" s="9"/>
       <c r="P127" s="9"/>
-      <c r="Q127" s="115"/>
+      <c r="Q127" s="103"/>
       <c r="R127" s="60" t="s">
         <v>29</v>
       </c>
@@ -23586,11 +23586,11 @@
       <c r="N146" s="9"/>
       <c r="O146" s="9"/>
       <c r="P146" s="9"/>
-      <c r="Q146" s="107" t="s">
+      <c r="Q146" s="109" t="s">
         <v>24</v>
       </c>
-      <c r="R146" s="108"/>
-      <c r="S146" s="109"/>
+      <c r="R146" s="110"/>
+      <c r="S146" s="111"/>
       <c r="T146" s="57"/>
       <c r="U146" s="77"/>
     </row>
@@ -23636,7 +23636,7 @@
       <c r="N148" s="9"/>
       <c r="O148" s="9"/>
       <c r="P148" s="9"/>
-      <c r="Q148" s="113" t="s">
+      <c r="Q148" s="101" t="s">
         <v>26</v>
       </c>
       <c r="R148" s="65"/>
@@ -23663,7 +23663,7 @@
       <c r="N149" s="9"/>
       <c r="O149" s="9"/>
       <c r="P149" s="9"/>
-      <c r="Q149" s="114"/>
+      <c r="Q149" s="102"/>
       <c r="R149" s="64" t="s">
         <v>27</v>
       </c>
@@ -23691,7 +23691,7 @@
       <c r="N150" s="9"/>
       <c r="O150" s="9"/>
       <c r="P150" s="9"/>
-      <c r="Q150" s="114"/>
+      <c r="Q150" s="102"/>
       <c r="R150" s="59" t="s">
         <v>28</v>
       </c>
@@ -23719,7 +23719,7 @@
       <c r="N151" s="9"/>
       <c r="O151" s="9"/>
       <c r="P151" s="9"/>
-      <c r="Q151" s="115"/>
+      <c r="Q151" s="103"/>
       <c r="R151" s="60" t="s">
         <v>29</v>
       </c>
@@ -23793,11 +23793,11 @@
       <c r="N154" s="9"/>
       <c r="O154" s="9"/>
       <c r="P154" s="9"/>
-      <c r="Q154" s="118" t="s">
+      <c r="Q154" s="106" t="s">
         <v>30</v>
       </c>
-      <c r="R154" s="119"/>
-      <c r="S154" s="120"/>
+      <c r="R154" s="107"/>
+      <c r="S154" s="108"/>
       <c r="T154" s="9"/>
       <c r="U154" s="10"/>
     </row>
@@ -23843,7 +23843,7 @@
       <c r="N156" s="9"/>
       <c r="O156" s="9"/>
       <c r="P156" s="9"/>
-      <c r="Q156" s="113" t="s">
+      <c r="Q156" s="101" t="s">
         <v>26</v>
       </c>
       <c r="R156" s="65"/>
@@ -23870,7 +23870,7 @@
       <c r="N157" s="9"/>
       <c r="O157" s="9"/>
       <c r="P157" s="9"/>
-      <c r="Q157" s="114"/>
+      <c r="Q157" s="102"/>
       <c r="R157" s="64" t="s">
         <v>27</v>
       </c>
@@ -23898,7 +23898,7 @@
       <c r="N158" s="9"/>
       <c r="O158" s="9"/>
       <c r="P158" s="9"/>
-      <c r="Q158" s="114"/>
+      <c r="Q158" s="102"/>
       <c r="R158" s="59" t="s">
         <v>28</v>
       </c>
@@ -23926,7 +23926,7 @@
       <c r="N159" s="9"/>
       <c r="O159" s="9"/>
       <c r="P159" s="9"/>
-      <c r="Q159" s="115"/>
+      <c r="Q159" s="103"/>
       <c r="R159" s="60" t="s">
         <v>29</v>
       </c>
@@ -24391,13 +24391,13 @@
       <c r="N179" s="9"/>
       <c r="O179" s="9"/>
       <c r="P179" s="9"/>
-      <c r="Q179" s="107" t="s">
+      <c r="Q179" s="109" t="s">
         <v>24</v>
       </c>
-      <c r="R179" s="108"/>
-      <c r="S179" s="108"/>
-      <c r="T179" s="108"/>
-      <c r="U179" s="109"/>
+      <c r="R179" s="110"/>
+      <c r="S179" s="110"/>
+      <c r="T179" s="110"/>
+      <c r="U179" s="111"/>
     </row>
     <row r="180" spans="1:21" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A180" s="8"/>
@@ -24417,12 +24417,12 @@
       <c r="O180" s="9"/>
       <c r="P180" s="55"/>
       <c r="Q180" s="58"/>
-      <c r="R180" s="110" t="s">
+      <c r="R180" s="112" t="s">
         <v>25</v>
       </c>
-      <c r="S180" s="111"/>
-      <c r="T180" s="111"/>
-      <c r="U180" s="112"/>
+      <c r="S180" s="113"/>
+      <c r="T180" s="113"/>
+      <c r="U180" s="114"/>
     </row>
     <row r="181" spans="1:21" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A181" s="8"/>
@@ -24441,7 +24441,7 @@
       <c r="N181" s="9"/>
       <c r="O181" s="9"/>
       <c r="P181" s="9"/>
-      <c r="Q181" s="113" t="s">
+      <c r="Q181" s="101" t="s">
         <v>26</v>
       </c>
       <c r="R181" s="65"/>
@@ -24472,7 +24472,7 @@
       <c r="N182" s="9"/>
       <c r="O182" s="9"/>
       <c r="P182" s="9"/>
-      <c r="Q182" s="114"/>
+      <c r="Q182" s="102"/>
       <c r="R182" s="64" t="s">
         <v>27</v>
       </c>
@@ -24506,7 +24506,7 @@
       <c r="N183" s="9"/>
       <c r="O183" s="9"/>
       <c r="P183" s="9"/>
-      <c r="Q183" s="114"/>
+      <c r="Q183" s="102"/>
       <c r="R183" s="59" t="s">
         <v>28</v>
       </c>
@@ -24540,7 +24540,7 @@
       <c r="N184" s="9"/>
       <c r="O184" s="9"/>
       <c r="P184" s="9"/>
-      <c r="Q184" s="115"/>
+      <c r="Q184" s="103"/>
       <c r="R184" s="60" t="s">
         <v>29</v>
       </c>
@@ -24643,13 +24643,13 @@
       <c r="N188" s="9"/>
       <c r="O188" s="9"/>
       <c r="P188" s="9"/>
-      <c r="Q188" s="107" t="s">
+      <c r="Q188" s="109" t="s">
         <v>30</v>
       </c>
-      <c r="R188" s="108"/>
-      <c r="S188" s="108"/>
-      <c r="T188" s="108"/>
-      <c r="U188" s="109"/>
+      <c r="R188" s="110"/>
+      <c r="S188" s="110"/>
+      <c r="T188" s="110"/>
+      <c r="U188" s="111"/>
     </row>
     <row r="189" spans="1:21" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A189" s="8"/>
@@ -24669,12 +24669,12 @@
       <c r="O189" s="9"/>
       <c r="P189" s="9"/>
       <c r="Q189" s="58"/>
-      <c r="R189" s="110" t="s">
+      <c r="R189" s="112" t="s">
         <v>25</v>
       </c>
-      <c r="S189" s="111"/>
-      <c r="T189" s="111"/>
-      <c r="U189" s="112"/>
+      <c r="S189" s="113"/>
+      <c r="T189" s="113"/>
+      <c r="U189" s="114"/>
     </row>
     <row r="190" spans="1:21" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A190" s="8"/>
@@ -24693,7 +24693,7 @@
       <c r="N190" s="9"/>
       <c r="O190" s="9"/>
       <c r="P190" s="9"/>
-      <c r="Q190" s="113" t="s">
+      <c r="Q190" s="101" t="s">
         <v>26</v>
       </c>
       <c r="R190" s="65"/>
@@ -24724,7 +24724,7 @@
       <c r="N191" s="9"/>
       <c r="O191" s="9"/>
       <c r="P191" s="9"/>
-      <c r="Q191" s="114"/>
+      <c r="Q191" s="102"/>
       <c r="R191" s="64" t="s">
         <v>27</v>
       </c>
@@ -24758,7 +24758,7 @@
       <c r="N192" s="9"/>
       <c r="O192" s="9"/>
       <c r="P192" s="9"/>
-      <c r="Q192" s="114"/>
+      <c r="Q192" s="102"/>
       <c r="R192" s="59" t="s">
         <v>28</v>
       </c>
@@ -24792,7 +24792,7 @@
       <c r="N193" s="9"/>
       <c r="O193" s="9"/>
       <c r="P193" s="9"/>
-      <c r="Q193" s="115"/>
+      <c r="Q193" s="103"/>
       <c r="R193" s="60" t="s">
         <v>29</v>
       </c>
@@ -26697,18 +26697,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="Q190:Q193"/>
-    <mergeCell ref="R48:S48"/>
-    <mergeCell ref="G73:I73"/>
-    <mergeCell ref="G74:I75"/>
-    <mergeCell ref="Q148:Q151"/>
-    <mergeCell ref="Q154:S154"/>
-    <mergeCell ref="Q156:Q159"/>
-    <mergeCell ref="Q181:Q184"/>
-    <mergeCell ref="Q179:U179"/>
-    <mergeCell ref="R180:U180"/>
-    <mergeCell ref="Q188:U188"/>
-    <mergeCell ref="R189:U189"/>
     <mergeCell ref="A3:U4"/>
     <mergeCell ref="Q146:S146"/>
     <mergeCell ref="Q122:U122"/>
@@ -26722,6 +26710,18 @@
     <mergeCell ref="Q115:Q118"/>
     <mergeCell ref="U48:W48"/>
     <mergeCell ref="U49:W50"/>
+    <mergeCell ref="Q190:Q193"/>
+    <mergeCell ref="R48:S48"/>
+    <mergeCell ref="G73:I73"/>
+    <mergeCell ref="G74:I75"/>
+    <mergeCell ref="Q148:Q151"/>
+    <mergeCell ref="Q154:S154"/>
+    <mergeCell ref="Q156:Q159"/>
+    <mergeCell ref="Q181:Q184"/>
+    <mergeCell ref="Q179:U179"/>
+    <mergeCell ref="R180:U180"/>
+    <mergeCell ref="Q188:U188"/>
+    <mergeCell ref="R189:U189"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -26846,10 +26846,10 @@
       <c r="O4" s="10"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="88" t="s">
+      <c r="A5" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="91">
+      <c r="B5" s="85">
         <v>9</v>
       </c>
       <c r="C5" s="44">
@@ -26866,13 +26866,13 @@
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="8"/>
-      <c r="I5" s="88" t="s">
+      <c r="I5" s="95" t="s">
         <v>8</v>
       </c>
       <c r="J5" s="47">
         <v>9</v>
       </c>
-      <c r="K5" s="94">
+      <c r="K5" s="88">
         <v>400</v>
       </c>
       <c r="L5" s="50" t="s">
@@ -26887,25 +26887,25 @@
       <c r="O5" s="10"/>
     </row>
     <row r="6" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="89"/>
-      <c r="B6" s="92"/>
+      <c r="A6" s="96"/>
+      <c r="B6" s="86"/>
       <c r="C6" s="21"/>
       <c r="D6" s="46"/>
       <c r="E6" s="9"/>
       <c r="F6" s="41"/>
       <c r="G6" s="9"/>
       <c r="H6" s="8"/>
-      <c r="I6" s="89"/>
+      <c r="I6" s="96"/>
       <c r="J6" s="52"/>
-      <c r="K6" s="95"/>
+      <c r="K6" s="89"/>
       <c r="L6" s="46"/>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
       <c r="O6" s="10"/>
     </row>
     <row r="7" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="89"/>
-      <c r="B7" s="92"/>
+      <c r="A7" s="96"/>
+      <c r="B7" s="86"/>
       <c r="C7" s="44">
         <v>400</v>
       </c>
@@ -26920,11 +26920,11 @@
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="8"/>
-      <c r="I7" s="89"/>
+      <c r="I7" s="96"/>
       <c r="J7" s="47">
         <v>14</v>
       </c>
-      <c r="K7" s="95"/>
+      <c r="K7" s="89"/>
       <c r="L7" s="50" t="s">
         <v>3</v>
       </c>
@@ -26937,25 +26937,25 @@
       <c r="O7" s="10"/>
     </row>
     <row r="8" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="89"/>
-      <c r="B8" s="92"/>
+      <c r="A8" s="96"/>
+      <c r="B8" s="86"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="F8" s="41"/>
       <c r="G8" s="9"/>
       <c r="H8" s="8"/>
-      <c r="I8" s="89"/>
+      <c r="I8" s="96"/>
       <c r="J8" s="48"/>
-      <c r="K8" s="95"/>
+      <c r="K8" s="89"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
       <c r="O8" s="10"/>
     </row>
     <row r="9" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="89"/>
-      <c r="B9" s="92"/>
+      <c r="A9" s="96"/>
+      <c r="B9" s="86"/>
       <c r="C9" s="44">
         <v>700</v>
       </c>
@@ -26970,11 +26970,11 @@
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="89"/>
+      <c r="I9" s="96"/>
       <c r="J9" s="47">
         <v>20</v>
       </c>
-      <c r="K9" s="95"/>
+      <c r="K9" s="89"/>
       <c r="L9" s="50" t="s">
         <v>3</v>
       </c>
@@ -26987,25 +26987,25 @@
       <c r="O9" s="10"/>
     </row>
     <row r="10" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="89"/>
-      <c r="B10" s="92"/>
+      <c r="A10" s="96"/>
+      <c r="B10" s="86"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="41"/>
       <c r="G10" s="9"/>
       <c r="H10" s="8"/>
-      <c r="I10" s="89"/>
+      <c r="I10" s="96"/>
       <c r="J10" s="48"/>
-      <c r="K10" s="95"/>
+      <c r="K10" s="89"/>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
       <c r="O10" s="10"/>
     </row>
     <row r="11" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="90"/>
-      <c r="B11" s="93"/>
+      <c r="A11" s="97"/>
+      <c r="B11" s="87"/>
       <c r="C11" s="44">
         <v>1024</v>
       </c>
@@ -27020,11 +27020,11 @@
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="8"/>
-      <c r="I11" s="89"/>
+      <c r="I11" s="96"/>
       <c r="J11" s="47">
         <v>25</v>
       </c>
-      <c r="K11" s="95"/>
+      <c r="K11" s="89"/>
       <c r="L11" s="50" t="s">
         <v>3</v>
       </c>
@@ -27045,9 +27045,9 @@
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="53"/>
-      <c r="I12" s="89"/>
+      <c r="I12" s="96"/>
       <c r="J12" s="48"/>
-      <c r="K12" s="95"/>
+      <c r="K12" s="89"/>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
@@ -27062,11 +27062,11 @@
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="90"/>
+      <c r="I13" s="97"/>
       <c r="J13" s="47">
         <v>30</v>
       </c>
-      <c r="K13" s="96"/>
+      <c r="K13" s="90"/>
       <c r="L13" s="50" t="s">
         <v>3</v>
       </c>

</xml_diff>